<commit_message>
Change text in the SELENIUM test case file
</commit_message>
<xml_diff>
--- a/SELENIUM test case.xlsx
+++ b/SELENIUM test case.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="273">
   <si>
     <t>Примітки</t>
   </si>
@@ -40,1917 +40,1924 @@
     <t>Тестові користувачі:</t>
   </si>
   <si>
+    <t>main user</t>
+  </si>
+  <si>
+    <t>логін alekslisergin
+пароль 1funny34qwer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тестові назви книг: </t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Dark Souls: Спокута. Том 1. Утрачена людяність</t>
+  </si>
+  <si>
+    <t>Funny</t>
+  </si>
+  <si>
+    <t>Bloodborne. Том 1. Глибина сну</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Виконавець</t>
+  </si>
+  <si>
+    <t>Назва</t>
+  </si>
+  <si>
+    <t>Кейс</t>
+  </si>
+  <si>
+    <t>Передумови</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Кроки перевірки</t>
+  </si>
+  <si>
+    <t>Очікуваний результат</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>Пріорітет</t>
+  </si>
+  <si>
+    <t>Automation Type</t>
+  </si>
+  <si>
+    <t>SER-01</t>
+  </si>
+  <si>
+    <t>Віталій</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Пошук книги </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>через панель пошуку на головній сторінці</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Main</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> доступна </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>в базі даних</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сайту</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Перейти на</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> головну сторінку</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сайта Книгарня-Є</t>
+    </r>
+  </si>
+  <si>
+    <t>Завантажуеться головна сторінка сайту</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Високий</t>
+  </si>
+  <si>
+    <t>automated</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на поле </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>пошуку,</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> щоб активувати його</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Випадає поле пошуку</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> зверху сторінки сайту</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Написати</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в випадющому полі </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>назву книги main</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">На сторінці відображаються товари, що </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>відповідають введеному запиту</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Клікнути </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>на книгу, що відобразилася</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> у результатах </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>пошуку на сайті.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Перехід на сторінку книги </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>книга main</t>
+    </r>
+  </si>
+  <si>
+    <t>LINK-01</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Перевірка переходів </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">за навігаційними посиланнями </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>в головному меню</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Користувач </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">знаходиться </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>на головній сторінці</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сайту</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Новинки"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Новинки книг в Книгарня «Є»</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Автори"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Автори</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> яка містить список авторів</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Видавництва"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Видавництво</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> яка містить список видавництв</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"ТОП книг"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ТОП книг в Книгарня «Є»</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Передпродажі"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Передпродажі книг</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>, для предзамовлень книг</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Акції"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Акції та знижки на книги</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Блог"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Блог</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Магазин і контакти"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Мережа книгарень</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натиснути</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Доставка і оплата"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Завантажуеться</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Доставка і оплата</t>
+    </r>
+  </si>
+  <si>
+    <t>ORD-01</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Додавання книги </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>до кошику з</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> зазначеною кількістю</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> екземплярів</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Знаходимо</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> через пошук  </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>книгу funny</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">, книга </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">доступна для замовлення, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>замовити</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> 3 шт</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Перейти на </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>сторінку книги Funny</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Сторінка</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> книги funny </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>завантажується</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">, відображаються </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>опис книги</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Натиснути кнопку </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Купити"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Книга funny </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>додається до кошику</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">, відкриваеться вікно </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Товар доданий у кошик"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Змніити </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>кількість</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> товару у кошику на 3</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> шт</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Кількість товару</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> змінюється на 3 шт</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">, відображається </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>оновлена сума</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> товарів в корзині</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Підтвердити замовлення, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>натиснувши</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> кнопку "</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Оформити замовлення</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">"        </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Відкривається </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>сторінка оформлення замовлення</t>
+    </r>
+  </si>
+  <si>
+    <t>Александр</t>
+  </si>
+  <si>
+    <t>Видалення товару з кошика</t>
+  </si>
+  <si>
+    <t>У кошику є товар в кількості 1шт</t>
+  </si>
+  <si>
+    <t>Перейти в кошик</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вдкриється вікно кошика </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Знайти та натиснути кнопку </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Видалити товар"</t>
+    </r>
+  </si>
+  <si>
+    <t>Товар буде успішно видалений з кошика</t>
+  </si>
+  <si>
+    <t>Оформлення замовлення</t>
+  </si>
+  <si>
+    <t>Товар доданий в кошик . Ми знаходимся на головынй сторінці</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перейти в кошик </t>
+  </si>
+  <si>
+    <t>В кошику буде товар , а нам запропонує оформити замовлення</t>
+  </si>
+  <si>
+    <t>Натиснуть на кнопку оформить замовлення</t>
+  </si>
+  <si>
+    <t>Відкриється вікно оформлення замовлення</t>
+  </si>
+  <si>
+    <t>Заповняємо всю інформацію необхідну інформацію</t>
+  </si>
+  <si>
+    <t>Успішне оформлення</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Вибираєм спосіб оплати </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Оплата картой "</t>
+    </r>
+  </si>
+  <si>
+    <t>Упішне оформлення</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Натискаєм на кнопку </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Підтвердить замовлення"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Відображається вікно про вдалу покупку товару. </t>
+  </si>
+  <si>
+    <t>LIKE-01</t>
+  </si>
+  <si>
+    <t>Вітлій</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Додавання книжки до</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> списку бажаних</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> товарів</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Користувач знаходиться </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>на сторінці книжки funny, к</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">ористувач </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>авторизований</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> на сайті</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Натиснути на кнопку </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Додати до списку бажаних"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Кнопка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Додати до списку бажаних"</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> змінюється на посилання із теском  </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"В списку побажань"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Натиснути на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"В списку побажань"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Відкривається </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>профіль користувача</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">, завантажується </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>список побажань</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Перевірити</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">, що книжка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>відображається у списку бажаних</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> товарів</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Книжка funny</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">присутня в списку бажаних </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>товарів у профілі</t>
+    </r>
+  </si>
+  <si>
+    <t>Проверка работы фильтров в ТОП книг</t>
+  </si>
+  <si>
+    <t>Знаходимся на головный сторінці</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Вибираєм пунк </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Топ Книги</t>
+    </r>
+  </si>
+  <si>
+    <t>Відкривається вікно ТОП книг в Книгарня «Є»</t>
+  </si>
+  <si>
+    <t>Середній</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Вибираєм наступні фільтри: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Тематика - Дитячі пригодницькі романи , Мова - Українська , Ціна - від Funny00 до Funny500</t>
+    </r>
+  </si>
+  <si>
+    <t>Біля кожно фільтру ставиться галочка .</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Натискаємо на кнопку</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> ОК-Застосувати</t>
+    </r>
+  </si>
+  <si>
+    <t>Відкривається сторінка з відповідним товаром</t>
+  </si>
+  <si>
+    <t>Авторизація користувача</t>
+  </si>
+  <si>
+    <t>Користувач зареєстрований на сатйі</t>
+  </si>
+  <si>
+    <t>Перейти на головну сторінку</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завантажуэться головна сторынка сайту </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> automated</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Натиснути на посилання </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Увійти або зареєструватися"</t>
+    </r>
+  </si>
+  <si>
+    <t>Відкриється вікно для заповнення логіну та пароля</t>
+  </si>
+  <si>
+    <t>Ввести логін та пароль</t>
+  </si>
+  <si>
+    <t>Відображуються символи</t>
+  </si>
+  <si>
+    <t>Натиснути на кнопку "Увійти"</t>
+  </si>
+  <si>
+    <t>Успішно авторизуємось на сайті</t>
+  </si>
+  <si>
+    <t>Підписуючись на розсилку</t>
+  </si>
+  <si>
+    <t>Знаходимся на головній сторінці</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Прогорнути сторінку донизу і натиснути на поле "</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Введіть свій e-mail"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Курсор блимає по середині рядка </t>
+  </si>
+  <si>
+    <t>Pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Низький </t>
+  </si>
+  <si>
+    <t>Заповнить поле</t>
+  </si>
+  <si>
+    <t>Успішне заповнення</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Натиснути на кнопку </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>"Підписатись"</t>
+    </r>
+  </si>
+  <si>
+    <t>На електрону адресу прийде лист з підтвердежнням</t>
+  </si>
+  <si>
+    <t>CON-01</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Пошук контактної інформації</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> магазину "Книгарня Є" </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>у місті Харків</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Користувач </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">знаходиться </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>на головній сторінці</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> сайту</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Натиснути на </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">"Магазини і контакти"  </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>в головному меню сайта</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Завантажуеться сторінка </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Мережа книгарень</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Вибрати</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> в Мережі книгарень місто </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Харків</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Відображається </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>контактна інформація</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> для магазину в місті </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Харків</t>
+    </r>
+  </si>
+  <si>
+    <t>Продивитися наявність контактної інформації</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">На сторінці відображаються: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>адреса, номер телефону, графік роботи</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://book-ye.com.ua/</t>
+    </r>
+  </si>
+  <si>
     <t>пользватель 1</t>
   </si>
   <si>
     <t>логін alekslisergin
 пароль 1234qwer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Тестові назви книг: </t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>Dark Souls: Спокута. Том 1. Утрачена людяність</t>
-  </si>
-  <si>
-    <t>Funy</t>
-  </si>
-  <si>
-    <t>Bloodborne. Том 1. Глибина сну</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Виконавець</t>
-  </si>
-  <si>
-    <t>Назва</t>
-  </si>
-  <si>
-    <t>Кейс</t>
-  </si>
-  <si>
-    <t>Передумови</t>
-  </si>
-  <si>
-    <t>№</t>
-  </si>
-  <si>
-    <t>Кроки перевірки</t>
-  </si>
-  <si>
-    <t>Очікуваний результат</t>
-  </si>
-  <si>
-    <t>Статус</t>
-  </si>
-  <si>
-    <t>Пріорітет</t>
-  </si>
-  <si>
-    <t>Automation Type</t>
-  </si>
-  <si>
-    <t>SER-01</t>
-  </si>
-  <si>
-    <t>Віталій</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Пошук книги </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>через панель пошуку на головній сторінці</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Main</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> доступна </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>в базі даних</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сайту</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>Перейти на</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> головну сторінку</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сайта Книгарня-Є</t>
-    </r>
-  </si>
-  <si>
-    <t>Завантажуеться головна сторінка сайту</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Високий</t>
-  </si>
-  <si>
-    <t>automated</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на поле </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>пошуку,</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> щоб активувати його</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>Випадає поле пошуку</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> зверху сторінки сайту</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Написати</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в випадющому полі </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>назву книги 1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">На сторінці відображаються товари, що </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>відповідають введеному запиту</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Клікнути </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>на книгу, що відобразилася</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> у результатах </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>пошуку на сайті.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Перехід на сторінку книги </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>книга 1</t>
-    </r>
-  </si>
-  <si>
-    <t>LINK-01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Перевірка переходів </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">за навігаційними посиланнями </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>в головному меню</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Користувач </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">знаходиться </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>на головній сторінці</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сайту</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Новинки"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Новинки книг в Книгарня «Є»</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Автори"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Автори</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> яка містить список авторів</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Видавництва"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Видавництво</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> яка містить список видавництв</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"ТОП книг"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ТОП книг в Книгарня «Є»</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Передпродажі"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Передпродажі книг</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>, для предзамовлень книг</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Акції"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Акції та знижки на книги</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Блог"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Блог</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Магазин і контакти"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Мережа книгарень</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натиснути</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Доставка і оплата"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Завантажуеться</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Доставка і оплата</t>
-    </r>
-  </si>
-  <si>
-    <t>ORD-01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Додавання книги </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>до кошику з</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> зазначеною кількістю</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> екземплярів</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Знаходимо</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> через пошук  </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>книгу 2</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">, книга </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">доступна для замовлення, </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>замовити</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> 3 шт</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Перейти на </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>сторінку книги 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Сторінка</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> книги 2 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>завантажується</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">, відображаються </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>опис книги</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Натиснути кнопку </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Купити"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Книга 2 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>додається до кошику</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">, відкриваеться вікно </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Товар доданий у кошик"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Змніити </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>кількість</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> товару у кошику на 3</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> шт</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>Кількість товару</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> змінюється на 3 шт</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">, відображається </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>оновлена сума</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> товарів в корзині</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Підтвердити замовлення, </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>натиснувши</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> кнопку "</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Оформити замовлення</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">"        </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Відкривається </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>сторінка оформлення замовлення</t>
-    </r>
-  </si>
-  <si>
-    <t>Александр</t>
-  </si>
-  <si>
-    <t>Видалення товару з кошика</t>
-  </si>
-  <si>
-    <t>У кошику є товар в кількості 1шт</t>
-  </si>
-  <si>
-    <t>Перейти в кошик</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Вдкриється вікно кошика </t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Знайти та натиснути кнопку </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Видалити товар"</t>
-    </r>
-  </si>
-  <si>
-    <t>Товар буде успішно видалений з кошика</t>
-  </si>
-  <si>
-    <t>Оформлення замовлення</t>
-  </si>
-  <si>
-    <t>Товар доданий в кошик . Ми знаходимся на головынй сторінці</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Перейти в кошик </t>
-  </si>
-  <si>
-    <t>В кошику буде товар , а нам запропонує оформити замовлення</t>
-  </si>
-  <si>
-    <t>Натиснуть на кнопку оформить замовлення</t>
-  </si>
-  <si>
-    <t>Відкриється вікно оформлення замовлення</t>
-  </si>
-  <si>
-    <t>Заповняємо всю інформацію необхідну інформацію</t>
-  </si>
-  <si>
-    <t>Успішне оформлення</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Вибираєм спосіб оплати </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Оплата картой "</t>
-    </r>
-  </si>
-  <si>
-    <t>Упішне оформлення</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Натискаєм на кнопку </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Підтвердить замовлення"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Відображається вікно про вдалу покупку товару. </t>
-  </si>
-  <si>
-    <t>LIKE-01</t>
-  </si>
-  <si>
-    <t>Вітлій</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>Додавання книжки до</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> списку бажаних</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> товарів</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Користувач знаходиться </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>на сторінці книжки 2, к</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">ористувач </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>авторизований</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> на сайті</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Натиснути на кнопку </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Додати до списку бажаних"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Кнопка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Додати до списку бажаних"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> змінюється на посилання із теском  </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"В списку побажань"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Натиснути на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"В списку побажань"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Відкривається </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>профіль користувача</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">, завантажується </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>список побажань</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Перевірити</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">, що книжка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>відображається у списку бажаних</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> товарів</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Книжка 2</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">присутня в списку бажаних </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>товарів у профілі</t>
-    </r>
-  </si>
-  <si>
-    <t>Проверка работы фильтров в ТОП книг</t>
-  </si>
-  <si>
-    <t>Знаходимся на головный сторінці</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Вибираєм пунк </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Топ Книги</t>
-    </r>
-  </si>
-  <si>
-    <t>Відкривається вікно ТОП книг в Книгарня «Є»</t>
-  </si>
-  <si>
-    <t>Середній</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Вибираєм наступні фільтри: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Тематика - Дитячі пригодницькі романи , Мова - Українська , Ціна - від 200 до 2500</t>
-    </r>
-  </si>
-  <si>
-    <t>Біля кожно фільтру ставиться галочка .</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="0"/>
-        <color theme="1"/>
-      </rPr>
-      <t>Натискаємо на кнопку</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> ОК-Застосувати</t>
-    </r>
-  </si>
-  <si>
-    <t>Відкривається сторінка з відповідним товаром</t>
-  </si>
-  <si>
-    <t>Авторизація користувача</t>
-  </si>
-  <si>
-    <t>Користувач зареєстрований на сатйі</t>
-  </si>
-  <si>
-    <t>Перейти на головну сторінку</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Завантажуэться головна сторынка сайту </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> automated</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Натиснути на посилання </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Увійти або зареєструватися"</t>
-    </r>
-  </si>
-  <si>
-    <t>Відкриється вікно для заповнення логіну та пароля</t>
-  </si>
-  <si>
-    <t>Ввести логін та пароль</t>
-  </si>
-  <si>
-    <t>Відображуються символи</t>
-  </si>
-  <si>
-    <t>Натиснути на кнопку "Увійти"</t>
-  </si>
-  <si>
-    <t>Успішно авторизуємось на сайті</t>
-  </si>
-  <si>
-    <t>Підписуючись на розсилку</t>
-  </si>
-  <si>
-    <t>Знаходимся на головній сторінці</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>Прогорнути сторінку донизу і натиснути на поле "</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Введіть свій e-mail"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Курсор блимає по середині рядка </t>
-  </si>
-  <si>
-    <t>Pas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Низький </t>
-  </si>
-  <si>
-    <t>Заповнить поле</t>
-  </si>
-  <si>
-    <t>Успішне заповнення</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Натиснути на кнопку </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>"Підписатись"</t>
-    </r>
-  </si>
-  <si>
-    <t>На електрону адресу прийде лист з підтвердежнням</t>
-  </si>
-  <si>
-    <t>CON-01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Пошук контактної інформації</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> магазину "Книгарня Є" </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>у місті Харків</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Користувач </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">знаходиться </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>на головній сторінці</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> сайту</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Натиснути на </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">"Магазини і контакти"  </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>в головному меню сайта</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Завантажуеться сторінка </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Мережа книгарень</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Вибрати</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> в Мережі книгарень місто </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Харків</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Відображається </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>контактна інформація</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> для магазину в місті </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Харків</t>
-    </r>
-  </si>
-  <si>
-    <t>Продивитися наявність контактної інформації</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">На сторінці відображаються: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>адреса, номер телефону, графік роботи</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr/>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://book-ye.com.ua/</t>
-    </r>
   </si>
   <si>
     <t>книга 1</t>
@@ -6765,11 +6772,11 @@
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="15" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -6797,7 +6804,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="15" t="s">
@@ -6814,7 +6821,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23" t="s">
@@ -6909,19 +6916,19 @@
         <v>24</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D10" s="28">
         <v>1.0</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F10" s="30">
         <v>1.0</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H10" s="32" t="s">
         <v>28</v>
@@ -6933,7 +6940,7 @@
         <v>30</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
@@ -6963,10 +6970,10 @@
         <v>2.0</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
@@ -6999,10 +7006,10 @@
         <v>3.0</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -7035,10 +7042,10 @@
         <v>4.0</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H13" s="38" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I13" s="35"/>
       <c r="J13" s="35"/>
@@ -7069,22 +7076,22 @@
         <v>24</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D14" s="27">
         <v>2.0</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F14" s="39">
         <v>1.0</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I14" s="33" t="s">
         <v>29</v>
@@ -7093,7 +7100,7 @@
         <v>30</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L14" s="26"/>
       <c r="M14" s="26"/>
@@ -7123,10 +7130,10 @@
         <v>2.0</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
@@ -7159,10 +7166,10 @@
         <v>3.0</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H16" s="41" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
@@ -7195,10 +7202,10 @@
         <v>4.0</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H17" s="41" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
@@ -7231,10 +7238,10 @@
         <v>5.0</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
@@ -7267,10 +7274,10 @@
         <v>6.0</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H19" s="41" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
@@ -7303,10 +7310,10 @@
         <v>7.0</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H20" s="41" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
@@ -7339,10 +7346,10 @@
         <v>8.0</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H21" s="41" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
@@ -7375,10 +7382,10 @@
         <v>9.0</v>
       </c>
       <c r="G22" s="42" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H22" s="43" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
@@ -7409,22 +7416,22 @@
         <v>24</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D23" s="27">
         <v>3.0</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F23" s="39">
         <v>1.0</v>
       </c>
       <c r="G23" s="44" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I23" s="33" t="s">
         <v>29</v>
@@ -7433,7 +7440,7 @@
         <v>30</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
@@ -7463,10 +7470,10 @@
         <v>2.0</v>
       </c>
       <c r="G24" s="41" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I24" s="34"/>
       <c r="J24" s="34"/>
@@ -7499,10 +7506,10 @@
         <v>3.0</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
@@ -7535,10 +7542,10 @@
         <v>4.0</v>
       </c>
       <c r="G26" s="43" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I26" s="35"/>
       <c r="J26" s="35"/>
@@ -7729,16 +7736,16 @@
         <v>5.0</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F32" s="39">
         <v>1.0</v>
       </c>
       <c r="G32" s="41" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H32" s="41" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="I32" s="27" t="s">
         <v>29</v>
@@ -7747,7 +7754,7 @@
         <v>30</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L32" s="26"/>
       <c r="M32" s="26"/>
@@ -7777,7 +7784,7 @@
         <v>2.0</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H33" s="32" t="s">
         <v>85</v>
@@ -7813,7 +7820,7 @@
         <v>3.0</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H34" s="32" t="s">
         <v>85</v>
@@ -7849,7 +7856,7 @@
         <v>4.0</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H35" s="32" t="s">
         <v>87</v>
@@ -7885,7 +7892,7 @@
         <v>5.0</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H36" s="37" t="s">
         <v>89</v>
@@ -7919,22 +7926,22 @@
         <v>91</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D37" s="27">
         <v>6.0</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F37" s="39">
         <v>1.0</v>
       </c>
       <c r="G37" s="41" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H37" s="41" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I37" s="27" t="s">
         <v>29</v>
@@ -7973,10 +7980,10 @@
         <v>2.0</v>
       </c>
       <c r="G38" s="32" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -8009,10 +8016,10 @@
         <v>3.0</v>
       </c>
       <c r="G39" s="37" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H39" s="37" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -8041,7 +8048,7 @@
         <v>70</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D40" s="27">
         <v>7.0</v>
@@ -8223,7 +8230,7 @@
         <v>104</v>
       </c>
       <c r="K45" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L45" s="26"/>
       <c r="M45" s="26"/>
@@ -8253,7 +8260,7 @@
         <v>2.0</v>
       </c>
       <c r="G46" s="57" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H46" s="57" t="s">
         <v>115</v>
@@ -8392,22 +8399,22 @@
         <v>24</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D55" s="27">
         <v>10.0</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F55" s="39">
         <v>1.0</v>
       </c>
       <c r="G55" s="41" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H55" s="41" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I55" s="27" t="s">
         <v>29</v>
@@ -8429,10 +8436,10 @@
         <v>2.0</v>
       </c>
       <c r="G56" s="57" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H56" s="57" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I56" s="34"/>
       <c r="J56" s="34"/>
@@ -8451,7 +8458,7 @@
         <v>137</v>
       </c>
       <c r="H57" s="63" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="I57" s="35"/>
       <c r="J57" s="35"/>
@@ -8642,16 +8649,16 @@
         <v>13</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D2" s="66" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E2" s="66" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="66" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G2" s="66" t="s">
         <v>16</v>
@@ -8691,31 +8698,31 @@
     </row>
     <row r="3">
       <c r="A3" s="69" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B3" s="69" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="69" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F3" s="69">
         <v>1.0</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H3" s="71" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="I3" s="71" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J3" s="72" t="s">
         <v>29</v>
@@ -8724,7 +8731,7 @@
         <v>104</v>
       </c>
       <c r="L3" s="74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M3" s="26"/>
       <c r="N3" s="26"/>
@@ -8746,31 +8753,31 @@
     </row>
     <row r="4">
       <c r="A4" s="69" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B4" s="69" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D4" s="69" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F4" s="69">
         <v>2.0</v>
       </c>
       <c r="G4" s="70" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H4" s="75" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I4" s="71" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J4" s="72" t="s">
         <v>29</v>
@@ -8779,7 +8786,7 @@
         <v>104</v>
       </c>
       <c r="L4" s="74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M4" s="26"/>
       <c r="N4" s="26"/>
@@ -8804,28 +8811,28 @@
         <v>23</v>
       </c>
       <c r="B5" s="76" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F5" s="76">
         <v>3.0</v>
       </c>
       <c r="G5" s="70" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H5" s="77" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I5" s="78" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="J5" s="73" t="s">
         <v>29</v>
@@ -8834,7 +8841,7 @@
         <v>104</v>
       </c>
       <c r="L5" s="74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M5" s="26"/>
       <c r="N5" s="26"/>
@@ -8856,40 +8863,40 @@
     </row>
     <row r="6">
       <c r="A6" s="76" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D6" s="76" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E6" s="70" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F6" s="76">
         <v>4.0</v>
       </c>
       <c r="G6" s="70" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H6" s="80" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="I6" s="78" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J6" s="73" t="s">
         <v>29</v>
       </c>
       <c r="K6" s="73" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="L6" s="74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M6" s="26"/>
       <c r="N6" s="26"/>
@@ -8911,38 +8918,38 @@
     </row>
     <row r="7">
       <c r="A7" s="76" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B7" s="76" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E7" s="70" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F7" s="76">
         <v>5.0</v>
       </c>
       <c r="G7" s="70" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H7" s="71" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="I7" s="71" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="J7" s="82"/>
       <c r="K7" s="82" t="s">
         <v>30</v>
       </c>
       <c r="L7" s="74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
@@ -8964,38 +8971,38 @@
     </row>
     <row r="8">
       <c r="A8" s="76" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B8" s="76" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C8" s="83" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D8" s="76" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E8" s="70" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F8" s="76">
         <v>6.0</v>
       </c>
       <c r="G8" s="70" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="H8" s="71" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I8" s="71" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="J8" s="82"/>
       <c r="K8" s="82" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M8" s="26"/>
       <c r="N8" s="26"/>
@@ -9017,40 +9024,40 @@
     </row>
     <row r="9">
       <c r="A9" s="69" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B9" s="69" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="69" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E9" s="70" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F9" s="69">
         <v>7.0</v>
       </c>
       <c r="G9" s="70" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="H9" s="78" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I9" s="78" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="J9" s="84" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="K9" s="84" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="L9" s="74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
@@ -9075,35 +9082,35 @@
         <v>59</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C10" s="69" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E10" s="70" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F10" s="69">
         <v>8.0</v>
       </c>
       <c r="G10" s="70" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="H10" s="78" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="I10" s="78" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="J10" s="85"/>
       <c r="K10" s="84" t="s">
         <v>30</v>
       </c>
       <c r="L10" s="74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -9125,38 +9132,38 @@
     </row>
     <row r="11">
       <c r="A11" s="69" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B11" s="69" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="69" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D11" s="69" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E11" s="86" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F11" s="69">
         <v>9.0</v>
       </c>
       <c r="G11" s="70" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="H11" s="78" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="I11" s="78" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="J11" s="85"/>
       <c r="K11" s="84" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="L11" s="74" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>

</xml_diff>